<commit_message>
January 12 / Make survey tool
</commit_message>
<xml_diff>
--- a/non_java_lesseons/테이블 설계.xlsx
+++ b/non_java_lesseons/테이블 설계.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkit\Desktop\jgd\workspace\non_java_lesseons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D33E5D-4F48-417E-8D3C-9BF56B7B338E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C907820D-1528-4133-A514-5E7E91F6778B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="28035" windowHeight="13005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="259">
   <si>
     <t>varchar2(50)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -928,6 +928,119 @@
   </si>
   <si>
     <t>varhchar2(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설문조사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문지 테이블</t>
+  </si>
+  <si>
+    <t>타이틀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필드명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제약조건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택내용1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택내용2</t>
+  </si>
+  <si>
+    <t>선택내용3</t>
+  </si>
+  <si>
+    <t>선택내용4</t>
+  </si>
+  <si>
+    <t>일련번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서비스여부(0, 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>question</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select2</t>
+  </si>
+  <si>
+    <t>select3</t>
+  </si>
+  <si>
+    <t>select4</t>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar2(4000)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar2(500)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default '0'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>응답 테이블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servey_no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servey_answer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1316,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X73"/>
+  <dimension ref="A1:X90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X72" sqref="X72"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2444,6 +2557,178 @@
       </c>
       <c r="K73" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>230</v>
+      </c>
+      <c r="B80" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>231</v>
+      </c>
+      <c r="B81" t="s">
+        <v>240</v>
+      </c>
+      <c r="C81" t="s">
+        <v>235</v>
+      </c>
+      <c r="D81" t="s">
+        <v>236</v>
+      </c>
+      <c r="E81" t="s">
+        <v>237</v>
+      </c>
+      <c r="F81" t="s">
+        <v>238</v>
+      </c>
+      <c r="G81" t="s">
+        <v>239</v>
+      </c>
+      <c r="H81" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>232</v>
+      </c>
+      <c r="B82" t="s">
+        <v>242</v>
+      </c>
+      <c r="C82" t="s">
+        <v>243</v>
+      </c>
+      <c r="D82" t="s">
+        <v>244</v>
+      </c>
+      <c r="E82" t="s">
+        <v>245</v>
+      </c>
+      <c r="F82" t="s">
+        <v>246</v>
+      </c>
+      <c r="G82" t="s">
+        <v>247</v>
+      </c>
+      <c r="H82" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>233</v>
+      </c>
+      <c r="B83" t="s">
+        <v>249</v>
+      </c>
+      <c r="C83" t="s">
+        <v>251</v>
+      </c>
+      <c r="D83" t="s">
+        <v>252</v>
+      </c>
+      <c r="E83" t="s">
+        <v>252</v>
+      </c>
+      <c r="F83" t="s">
+        <v>252</v>
+      </c>
+      <c r="G83" t="s">
+        <v>252</v>
+      </c>
+      <c r="H83" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>234</v>
+      </c>
+      <c r="B84" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" t="s">
+        <v>250</v>
+      </c>
+      <c r="E84" t="s">
+        <v>250</v>
+      </c>
+      <c r="F84" t="s">
+        <v>250</v>
+      </c>
+      <c r="G84" t="s">
+        <v>250</v>
+      </c>
+      <c r="H84" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>231</v>
+      </c>
+      <c r="B87" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>232</v>
+      </c>
+      <c r="B88" t="s">
+        <v>242</v>
+      </c>
+      <c r="C88" t="s">
+        <v>257</v>
+      </c>
+      <c r="D88" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>233</v>
+      </c>
+      <c r="B89" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" t="s">
+        <v>249</v>
+      </c>
+      <c r="D89" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>234</v>
+      </c>
+      <c r="B90" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" t="s">
+        <v>250</v>
+      </c>
+      <c r="D90" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>